<commit_message>
Aug 3, 2014 1:48 PM
</commit_message>
<xml_diff>
--- a/dissertaion progress.xlsx
+++ b/dissertaion progress.xlsx
@@ -141,7 +141,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -149,12 +149,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -164,19 +175,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -510,7 +523,7 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -522,8 +535,8 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7">
-        <v>11763</v>
+      <c r="B2" s="4">
+        <v>14169</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -538,38 +551,42 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="5">
         <f>B2/B3</f>
-        <v>0.49012499999999998</v>
+        <v>0.59037499999999998</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="D9" s="9">
+      <c r="B9" s="10"/>
+      <c r="D9" s="6">
         <f>B2</f>
-        <v>11763</v>
-      </c>
-      <c r="E9" s="4">
+        <v>14169</v>
+      </c>
+      <c r="E9" s="7">
         <f>B2</f>
-        <v>11763</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
+        <v>14169</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
       <c r="H9">
         <f>B3</f>
         <v>24000</v>
       </c>
     </row>
     <row r="11" spans="1:8">
+      <c r="B11" s="4">
+        <v>14028</v>
+      </c>
       <c r="D11" s="1">
         <f>B2/B3</f>
-        <v>0.49012499999999998</v>
-      </c>
-      <c r="E11" s="4">
+        <v>0.59037499999999998</v>
+      </c>
+      <c r="E11" s="7">
         <f>B4*100</f>
-        <v>49.012499999999996</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
+        <v>59.037500000000001</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="1">
         <f>B3/B3</f>
         <v>1</v>

</xml_diff>

<commit_message>
Aug 4, 2014 10:49 PM
</commit_message>
<xml_diff>
--- a/dissertaion progress.xlsx
+++ b/dissertaion progress.xlsx
@@ -527,7 +527,7 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>15162</v>
+        <v>15560</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -557,18 +557,18 @@
       </c>
       <c r="B4" s="5">
         <f>B2/B3</f>
-        <v>0.63175000000000003</v>
+        <v>0.64833333333333332</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="B9" s="10"/>
       <c r="D9" s="6">
         <f>B2</f>
-        <v>15162</v>
+        <v>15560</v>
       </c>
       <c r="E9" s="7">
         <f>B2</f>
-        <v>15162</v>
+        <v>15560</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
@@ -583,11 +583,11 @@
       </c>
       <c r="D11" s="1">
         <f>B2/B3</f>
-        <v>0.63175000000000003</v>
+        <v>0.64833333333333332</v>
       </c>
       <c r="E11" s="7">
         <f>B4*100</f>
-        <v>63.175000000000004</v>
+        <v>64.833333333333329</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="9"/>

</xml_diff>

<commit_message>
Aug 6, 2014 7:57 PM
</commit_message>
<xml_diff>
--- a/dissertaion progress.xlsx
+++ b/dissertaion progress.xlsx
@@ -168,6 +168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -177,7 +178,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -527,7 +527,7 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>15560</v>
+        <v>16242</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -557,40 +557,40 @@
       </c>
       <c r="B4" s="5">
         <f>B2/B3</f>
-        <v>0.64833333333333332</v>
+        <v>0.67674999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="B9" s="10"/>
+      <c r="B9" s="7"/>
       <c r="D9" s="6">
         <f>B2</f>
-        <v>15560</v>
-      </c>
-      <c r="E9" s="7">
+        <v>16242</v>
+      </c>
+      <c r="E9" s="8">
         <f>B2</f>
-        <v>15560</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
+        <v>16242</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10"/>
       <c r="H9">
         <f>B3</f>
         <v>24000</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="B11" s="4">
-        <v>14697</v>
+      <c r="B11" s="7">
+        <v>16192</v>
       </c>
       <c r="D11" s="1">
         <f>B2/B3</f>
-        <v>0.64833333333333332</v>
-      </c>
-      <c r="E11" s="7">
+        <v>0.67674999999999996</v>
+      </c>
+      <c r="E11" s="8">
         <f>B4*100</f>
-        <v>64.833333333333329</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
+        <v>67.674999999999997</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="10"/>
       <c r="H11" s="1">
         <f>B3/B3</f>
         <v>1</v>

</xml_diff>

<commit_message>
Aug 9, 2014 9:26 PM
</commit_message>
<xml_diff>
--- a/dissertaion progress.xlsx
+++ b/dissertaion progress.xlsx
@@ -527,7 +527,7 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>16242</v>
+        <v>17344</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -548,7 +548,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>24000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -557,37 +557,42 @@
       </c>
       <c r="B4" s="5">
         <f>B2/B3</f>
-        <v>0.67674999999999996</v>
+        <v>0.86719999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="C7">
+        <v>21000</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="B9" s="7"/>
       <c r="D9" s="6">
         <f>B2</f>
-        <v>16242</v>
+        <v>17344</v>
       </c>
       <c r="E9" s="8">
         <f>B2</f>
-        <v>16242</v>
+        <v>17344</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="10"/>
       <c r="H9">
         <f>B3</f>
-        <v>24000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="B11" s="7">
-        <v>16192</v>
+        <v>16942</v>
       </c>
       <c r="D11" s="1">
         <f>B2/B3</f>
-        <v>0.67674999999999996</v>
+        <v>0.86719999999999997</v>
       </c>
       <c r="E11" s="8">
         <f>B4*100</f>
-        <v>67.674999999999997</v>
+        <v>86.72</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="10"/>
@@ -602,7 +607,7 @@
     <mergeCell ref="E11:G11"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:G9">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="&quot;0$B$3&quot;"/>
@@ -614,7 +619,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="$B$3"/>
@@ -626,7 +631,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="24000"/>
@@ -638,9 +643,33 @@
         </ext>
       </extLst>
     </cfRule>
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="20000"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{746474BA-CAAE-FC49-A76D-009002375598}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="$H$9"/>
+        <color rgb="FFFF0000"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2CAA8BA5-3009-DD41-8970-A9AA30847C8F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:G11">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -652,7 +681,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -707,6 +736,30 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
+          <x14:cfRule type="dataBar" id="{746474BA-CAAE-FC49-A76D-009002375598}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>20000</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <x14:cfRule type="dataBar" id="{2CAA8BA5-3009-DD41-8970-A9AA30847C8F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>$H$9</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
           <xm:sqref>E9:G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">

</xml_diff>

<commit_message>
Aug 11, 2014 6:25 PM
</commit_message>
<xml_diff>
--- a/dissertaion progress.xlsx
+++ b/dissertaion progress.xlsx
@@ -527,7 +527,7 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>17344</v>
+        <v>18007</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -557,7 +557,7 @@
       </c>
       <c r="B4" s="5">
         <f>B2/B3</f>
-        <v>0.86719999999999997</v>
+        <v>0.90034999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -569,11 +569,11 @@
       <c r="B9" s="7"/>
       <c r="D9" s="6">
         <f>B2</f>
-        <v>17344</v>
+        <v>18007</v>
       </c>
       <c r="E9" s="8">
         <f>B2</f>
-        <v>17344</v>
+        <v>18007</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="10"/>
@@ -588,11 +588,11 @@
       </c>
       <c r="D11" s="1">
         <f>B2/B3</f>
-        <v>0.86719999999999997</v>
+        <v>0.90034999999999998</v>
       </c>
       <c r="E11" s="8">
         <f>B4*100</f>
-        <v>86.72</v>
+        <v>90.034999999999997</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="10"/>

</xml_diff>

<commit_message>
Aug 13, 2014 1:40 PM
</commit_message>
<xml_diff>
--- a/dissertaion progress.xlsx
+++ b/dissertaion progress.xlsx
@@ -527,7 +527,7 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>18007</v>
+        <v>18631</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -557,7 +557,7 @@
       </c>
       <c r="B4" s="5">
         <f>B2/B3</f>
-        <v>0.90034999999999998</v>
+        <v>0.93154999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -569,11 +569,11 @@
       <c r="B9" s="7"/>
       <c r="D9" s="6">
         <f>B2</f>
-        <v>18007</v>
+        <v>18631</v>
       </c>
       <c r="E9" s="8">
         <f>B2</f>
-        <v>18007</v>
+        <v>18631</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="10"/>
@@ -588,11 +588,11 @@
       </c>
       <c r="D11" s="1">
         <f>B2/B3</f>
-        <v>0.90034999999999998</v>
+        <v>0.93154999999999999</v>
       </c>
       <c r="E11" s="8">
         <f>B4*100</f>
-        <v>90.034999999999997</v>
+        <v>93.155000000000001</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="10"/>

</xml_diff>

<commit_message>
Aug 14, 2014 8:08 PM
</commit_message>
<xml_diff>
--- a/dissertaion progress.xlsx
+++ b/dissertaion progress.xlsx
@@ -527,7 +527,7 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>18631</v>
+        <v>19358</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -557,7 +557,7 @@
       </c>
       <c r="B4" s="5">
         <f>B2/B3</f>
-        <v>0.93154999999999999</v>
+        <v>0.96789999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -569,11 +569,11 @@
       <c r="B9" s="7"/>
       <c r="D9" s="6">
         <f>B2</f>
-        <v>18631</v>
+        <v>19358</v>
       </c>
       <c r="E9" s="8">
         <f>B2</f>
-        <v>18631</v>
+        <v>19358</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="10"/>
@@ -588,11 +588,11 @@
       </c>
       <c r="D11" s="1">
         <f>B2/B3</f>
-        <v>0.93154999999999999</v>
+        <v>0.96789999999999998</v>
       </c>
       <c r="E11" s="8">
         <f>B4*100</f>
-        <v>93.155000000000001</v>
+        <v>96.789999999999992</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="10"/>

</xml_diff>